<commit_message>
Subject code update, course code acc
</commit_message>
<xml_diff>
--- a/ocr_scripts/subject_code.xlsx
+++ b/ocr_scripts/subject_code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshu\Documents\GitHub\Admissions-Smart-OCR\ocr_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45EE936-1FC9-4A99-9BEB-FF2F46AC7BB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EE33FE-979F-4F2E-BFE1-1D8016AC68B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-360" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subject Areas" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="685">
   <si>
     <t>Subject code</t>
   </si>
@@ -1956,31 +1956,139 @@
     <t>ENGLISH LITERATURE AND COMPOSITION</t>
   </si>
   <si>
-    <t>ALGEBRA 1 PART 2 (must take part 1 and 2 for 1 unit) give .5 credits</t>
-  </si>
-  <si>
-    <t>ALGEBRA 1 PART 1(must take part 1 and 2 for 1 unit) give .5 credits</t>
-  </si>
-  <si>
-    <t>ELEFUNS</t>
-  </si>
-  <si>
-    <t>INTERGRATED MATH 4</t>
-  </si>
-  <si>
-    <t>INTERGRATED MATH 3</t>
-  </si>
-  <si>
-    <t>INTERGRATED MATH 2</t>
-  </si>
-  <si>
-    <t>INTERGRATED MATH 1</t>
-  </si>
-  <si>
     <t>AGRCULT</t>
   </si>
   <si>
     <t>AGRICULTURE</t>
+  </si>
+  <si>
+    <t>BANK</t>
+  </si>
+  <si>
+    <t>BANKING</t>
+  </si>
+  <si>
+    <t>BANKFIN</t>
+  </si>
+  <si>
+    <t>BANKING AND FINANCE</t>
+  </si>
+  <si>
+    <t>COMKB</t>
+  </si>
+  <si>
+    <t>COMPUTER KEYBOARDING</t>
+  </si>
+  <si>
+    <t>ALGEBRA 1 PART 1</t>
+  </si>
+  <si>
+    <t>ALGEBRA 1 PART 2</t>
+  </si>
+  <si>
+    <t>INTEGRATED MATH 1</t>
+  </si>
+  <si>
+    <t>INTEGRATED MATH 2</t>
+  </si>
+  <si>
+    <t>INTEGRATED MATH 3</t>
+  </si>
+  <si>
+    <t>INTEGRATED MATH 4</t>
+  </si>
+  <si>
+    <t>ELEFUN</t>
+  </si>
+  <si>
+    <t>SAT</t>
+  </si>
+  <si>
+    <t>ACT/SAT PREPARATION</t>
+  </si>
+  <si>
+    <t>ARCH</t>
+  </si>
+  <si>
+    <t>ARCHITECTURE</t>
+  </si>
+  <si>
+    <t>CULN</t>
+  </si>
+  <si>
+    <t>CULINARY ARTS</t>
+  </si>
+  <si>
+    <t>DRIVED</t>
+  </si>
+  <si>
+    <t>DRIVERS EDUCATION</t>
+  </si>
+  <si>
+    <t>FRSH</t>
+  </si>
+  <si>
+    <t>FRESHMAN SEMINAR</t>
+  </si>
+  <si>
+    <t>INTERN</t>
+  </si>
+  <si>
+    <t>INTERNSHIP</t>
+  </si>
+  <si>
+    <t>JROTC</t>
+  </si>
+  <si>
+    <t>JUNIOR ROTC / ROTC</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>SEMINAR</t>
+  </si>
+  <si>
+    <t>YRBOOK</t>
+  </si>
+  <si>
+    <t>YEARBOOK</t>
+  </si>
+  <si>
+    <t>OT_OTH</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>HLTH</t>
+  </si>
+  <si>
+    <t>HEALTH EDUCATION</t>
+  </si>
+  <si>
+    <t>PE1</t>
+  </si>
+  <si>
+    <t>PHYSICAL EDUCATION</t>
+  </si>
+  <si>
+    <t>PEHLTH</t>
+  </si>
+  <si>
+    <t>PHYSICAL EDUCATION AND HEALTH</t>
+  </si>
+  <si>
+    <t>SPORT</t>
+  </si>
+  <si>
+    <t>VARSITY SPORT</t>
+  </si>
+  <si>
+    <t>PE_OTH</t>
+  </si>
+  <si>
+    <t>OTHER PHYSICAL EDUCATION</t>
   </si>
 </sst>
 </file>
@@ -2014,19 +2122,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2041,8 +2150,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -2055,22 +2168,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal 1" xfId="5" xr:uid="{1AE2D8F0-FD88-4232-8830-74E81B09C55A}"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{2A1E1316-805E-4E20-89E1-DCD639E4D076}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2465,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C326"/>
+  <dimension ref="A1:C333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="C334" sqref="C334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,15 +2611,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2505,10 +2627,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2516,10 +2638,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2527,10 +2649,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>642</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>46</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2538,10 +2660,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>644</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>42</v>
+        <v>645</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2549,10 +2671,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2571,10 +2693,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2582,10 +2704,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2593,10 +2715,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2604,10 +2726,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2615,10 +2737,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2626,10 +2748,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2637,10 +2759,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2648,10 +2770,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2659,10 +2781,10 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2670,32 +2792,32 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2703,10 +2825,10 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2714,10 +2836,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2725,10 +2847,10 @@
         <v>12</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>67</v>
+        <v>646</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>68</v>
+        <v>647</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2736,10 +2858,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2747,76 +2869,76 @@
         <v>12</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="B29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="B30" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>105</v>
+      <c r="B31" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2824,10 +2946,10 @@
         <v>2</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2835,10 +2957,10 @@
         <v>2</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2846,21 +2968,21 @@
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>85</v>
+      <c r="B35" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2868,32 +2990,32 @@
         <v>2</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>107</v>
+      <c r="B37" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>103</v>
+      <c r="B38" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2908,25 +3030,25 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>94</v>
+      <c r="B40" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>636</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>637</v>
+      <c r="B41" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2941,91 +3063,91 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>81</v>
+      <c r="B43" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>79</v>
+      <c r="B44" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>77</v>
+      <c r="B45" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>75</v>
+      <c r="B46" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>495</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>495</v>
+      <c r="B50" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3033,10 +3155,10 @@
         <v>18</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3044,21 +3166,21 @@
         <v>18</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>496</v>
+      <c r="B53" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3066,10 +3188,10 @@
         <v>18</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3077,21 +3199,21 @@
         <v>18</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>125</v>
+      <c r="B56" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3099,131 +3221,131 @@
         <v>18</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B61" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C61" s="7" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B62" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C62" s="7" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B63" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C63" s="7" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B64" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C64" s="7" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B65" s="7" t="s">
         <v>505</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C65" s="7" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B66" s="7" t="s">
         <v>507</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C66" s="7" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B67" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C67" s="7" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B68" s="7" t="s">
         <v>511</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C68" s="7" t="s">
         <v>512</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -3231,10 +3353,10 @@
         <v>18</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3242,10 +3364,10 @@
         <v>18</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3253,10 +3375,10 @@
         <v>18</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3264,43 +3386,43 @@
         <v>18</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>415</v>
+        <v>138</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>416</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>413</v>
+        <v>128</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>414</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>412</v>
+      <c r="A75" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3308,10 +3430,10 @@
         <v>10</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>409</v>
+        <v>375</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>410</v>
+        <v>376</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3319,10 +3441,10 @@
         <v>10</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>408</v>
+        <v>378</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3330,10 +3452,10 @@
         <v>10</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>405</v>
+        <v>379</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>406</v>
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3341,10 +3463,10 @@
         <v>10</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>404</v>
+        <v>382</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3352,10 +3474,10 @@
         <v>10</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -3363,10 +3485,10 @@
         <v>10</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>399</v>
+        <v>385</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>400</v>
+        <v>386</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -3374,10 +3496,10 @@
         <v>10</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>397</v>
+        <v>140</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>398</v>
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -3385,10 +3507,10 @@
         <v>10</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>395</v>
+        <v>142</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>396</v>
+        <v>143</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -3396,10 +3518,10 @@
         <v>10</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>393</v>
+        <v>144</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>394</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3407,10 +3529,10 @@
         <v>10</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>391</v>
+        <v>146</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>392</v>
+        <v>147</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3418,10 +3540,10 @@
         <v>10</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>389</v>
+        <v>148</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>390</v>
+        <v>149</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -3429,10 +3551,10 @@
         <v>10</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>387</v>
+        <v>150</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>388</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3440,10 +3562,10 @@
         <v>10</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>385</v>
+        <v>152</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>386</v>
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3451,10 +3573,10 @@
         <v>10</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>383</v>
+        <v>154</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>384</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3462,10 +3584,10 @@
         <v>10</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>381</v>
+        <v>156</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>382</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -3473,10 +3595,10 @@
         <v>10</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>379</v>
+        <v>158</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>380</v>
+        <v>159</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3484,10 +3606,10 @@
         <v>10</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>377</v>
+        <v>160</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>378</v>
+        <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3495,10 +3617,10 @@
         <v>10</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>375</v>
+        <v>162</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>376</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3506,10 +3628,10 @@
         <v>10</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>373</v>
+        <v>164</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>374</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3517,10 +3639,10 @@
         <v>10</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>371</v>
+        <v>166</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>372</v>
+        <v>167</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3528,10 +3650,10 @@
         <v>10</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>369</v>
+        <v>168</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>370</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3539,10 +3661,10 @@
         <v>10</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>367</v>
+        <v>170</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>368</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3550,10 +3672,10 @@
         <v>10</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>365</v>
+        <v>172</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>366</v>
+        <v>173</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3561,10 +3683,10 @@
         <v>10</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>363</v>
+        <v>174</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>364</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3572,10 +3694,10 @@
         <v>10</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>361</v>
+        <v>176</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>362</v>
+        <v>177</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -3583,10 +3705,10 @@
         <v>10</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>359</v>
+        <v>178</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>360</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3594,10 +3716,10 @@
         <v>10</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>357</v>
+        <v>180</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>358</v>
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3605,10 +3727,10 @@
         <v>10</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>355</v>
+        <v>182</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>356</v>
+        <v>182</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3616,10 +3738,10 @@
         <v>10</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>353</v>
+        <v>183</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>354</v>
+        <v>184</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3627,10 +3749,10 @@
         <v>10</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>351</v>
+        <v>185</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>352</v>
+        <v>186</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3638,10 +3760,10 @@
         <v>10</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>349</v>
+        <v>187</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>350</v>
+        <v>188</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3649,10 +3771,10 @@
         <v>10</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>347</v>
+        <v>189</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>348</v>
+        <v>190</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -3660,10 +3782,10 @@
         <v>10</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>343</v>
+        <v>191</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>344</v>
+        <v>192</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3671,10 +3793,10 @@
         <v>10</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>341</v>
+        <v>193</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>342</v>
+        <v>194</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -3682,10 +3804,10 @@
         <v>10</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>339</v>
+        <v>195</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>340</v>
+        <v>196</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3693,10 +3815,10 @@
         <v>10</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>337</v>
+        <v>197</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>338</v>
+        <v>198</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3704,10 +3826,10 @@
         <v>10</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>335</v>
+        <v>199</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>336</v>
+        <v>200</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3715,10 +3837,10 @@
         <v>10</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>333</v>
+        <v>201</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>334</v>
+        <v>202</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3726,10 +3848,10 @@
         <v>10</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>331</v>
+        <v>203</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>332</v>
+        <v>204</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3737,10 +3859,10 @@
         <v>10</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>329</v>
+        <v>205</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>330</v>
+        <v>206</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3748,10 +3870,10 @@
         <v>10</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>327</v>
+        <v>207</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>328</v>
+        <v>208</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -3759,10 +3881,10 @@
         <v>10</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>325</v>
+        <v>209</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>326</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -3770,10 +3892,10 @@
         <v>10</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>323</v>
+        <v>211</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>324</v>
+        <v>212</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -3781,10 +3903,10 @@
         <v>10</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>321</v>
+        <v>213</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>322</v>
+        <v>214</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -3792,10 +3914,10 @@
         <v>10</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>319</v>
+        <v>215</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>320</v>
+        <v>216</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -3803,10 +3925,10 @@
         <v>10</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>317</v>
+        <v>217</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>318</v>
+        <v>218</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -3814,10 +3936,10 @@
         <v>10</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>315</v>
+        <v>219</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>316</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -3825,10 +3947,10 @@
         <v>10</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>313</v>
+        <v>221</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>314</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -3836,10 +3958,10 @@
         <v>10</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>311</v>
+        <v>223</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>312</v>
+        <v>224</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -3847,10 +3969,10 @@
         <v>10</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>309</v>
+        <v>225</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>310</v>
+        <v>226</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -3858,10 +3980,10 @@
         <v>10</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>307</v>
+        <v>227</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>308</v>
+        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -3869,10 +3991,10 @@
         <v>10</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>305</v>
+        <v>229</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>306</v>
+        <v>230</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -3880,10 +4002,10 @@
         <v>10</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>303</v>
+        <v>231</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>304</v>
+        <v>232</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -3891,10 +4013,10 @@
         <v>10</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>301</v>
+        <v>233</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>302</v>
+        <v>234</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -3902,10 +4024,10 @@
         <v>10</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>299</v>
+        <v>235</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>300</v>
+        <v>236</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -3913,10 +4035,10 @@
         <v>10</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>297</v>
+        <v>237</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>298</v>
+        <v>238</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -3924,10 +4046,10 @@
         <v>10</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>295</v>
+        <v>239</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>296</v>
+        <v>240</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -3935,10 +4057,10 @@
         <v>10</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>293</v>
+        <v>241</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>294</v>
+        <v>242</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -3946,10 +4068,10 @@
         <v>10</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -3957,10 +4079,10 @@
         <v>10</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>289</v>
+        <v>245</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>290</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -3968,10 +4090,10 @@
         <v>10</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>287</v>
+        <v>247</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>288</v>
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -3979,10 +4101,10 @@
         <v>10</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -3990,10 +4112,10 @@
         <v>10</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -4001,10 +4123,10 @@
         <v>10</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -4012,10 +4134,10 @@
         <v>10</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -4023,10 +4145,10 @@
         <v>10</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>277</v>
+        <v>257</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -4034,10 +4156,10 @@
         <v>10</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -4045,10 +4167,10 @@
         <v>10</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -4056,10 +4178,10 @@
         <v>10</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -4067,10 +4189,10 @@
         <v>10</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -4089,10 +4211,10 @@
         <v>10</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -4100,10 +4222,10 @@
         <v>10</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -4111,10 +4233,10 @@
         <v>10</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -4122,10 +4244,10 @@
         <v>10</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -4133,10 +4255,10 @@
         <v>10</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -4144,10 +4266,10 @@
         <v>10</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -4155,10 +4277,10 @@
         <v>10</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -4166,10 +4288,10 @@
         <v>10</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>251</v>
+        <v>283</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -4177,10 +4299,10 @@
         <v>10</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>249</v>
+        <v>285</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>250</v>
+        <v>286</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -4188,10 +4310,10 @@
         <v>10</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>247</v>
+        <v>287</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -4199,10 +4321,10 @@
         <v>10</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>245</v>
+        <v>289</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>246</v>
+        <v>290</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -4210,10 +4332,10 @@
         <v>10</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>243</v>
+        <v>291</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -4221,10 +4343,10 @@
         <v>10</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>241</v>
+        <v>293</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>242</v>
+        <v>294</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -4232,10 +4354,10 @@
         <v>10</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>239</v>
+        <v>295</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>240</v>
+        <v>296</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -4243,10 +4365,10 @@
         <v>10</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>237</v>
+        <v>297</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>238</v>
+        <v>298</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -4254,10 +4376,10 @@
         <v>10</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>235</v>
+        <v>299</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>236</v>
+        <v>300</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -4265,10 +4387,10 @@
         <v>10</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>233</v>
+        <v>301</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>234</v>
+        <v>302</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -4276,10 +4398,10 @@
         <v>10</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>231</v>
+        <v>303</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>232</v>
+        <v>304</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -4287,10 +4409,10 @@
         <v>10</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>230</v>
+        <v>306</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -4298,10 +4420,10 @@
         <v>10</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>227</v>
+        <v>307</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>228</v>
+        <v>308</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -4309,10 +4431,10 @@
         <v>10</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>225</v>
+        <v>309</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>226</v>
+        <v>310</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -4320,10 +4442,10 @@
         <v>10</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>223</v>
+        <v>311</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>224</v>
+        <v>312</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -4331,10 +4453,10 @@
         <v>10</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>221</v>
+        <v>313</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>222</v>
+        <v>314</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -4342,10 +4464,10 @@
         <v>10</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>219</v>
+        <v>315</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>220</v>
+        <v>316</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -4353,10 +4475,10 @@
         <v>10</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>217</v>
+        <v>317</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>218</v>
+        <v>318</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -4364,10 +4486,10 @@
         <v>10</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>215</v>
+        <v>319</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>216</v>
+        <v>320</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -4375,10 +4497,10 @@
         <v>10</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>214</v>
+        <v>322</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -4386,10 +4508,10 @@
         <v>10</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>211</v>
+        <v>323</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>212</v>
+        <v>324</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -4397,10 +4519,10 @@
         <v>10</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>209</v>
+        <v>325</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>210</v>
+        <v>326</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -4408,10 +4530,10 @@
         <v>10</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>207</v>
+        <v>327</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>208</v>
+        <v>328</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -4419,10 +4541,10 @@
         <v>10</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>205</v>
+        <v>329</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>206</v>
+        <v>330</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -4430,10 +4552,10 @@
         <v>10</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>203</v>
+        <v>331</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>204</v>
+        <v>332</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -4441,10 +4563,10 @@
         <v>10</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>201</v>
+        <v>333</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>202</v>
+        <v>334</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -4452,10 +4574,10 @@
         <v>10</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>199</v>
+        <v>335</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>200</v>
+        <v>336</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -4463,10 +4585,10 @@
         <v>10</v>
       </c>
       <c r="B181" s="4" t="s">
-        <v>197</v>
+        <v>337</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>198</v>
+        <v>338</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -4474,10 +4596,10 @@
         <v>10</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -4485,10 +4607,10 @@
         <v>10</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>195</v>
+        <v>341</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>196</v>
+        <v>342</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -4496,10 +4618,10 @@
         <v>10</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>193</v>
+        <v>343</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>194</v>
+        <v>344</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -4507,10 +4629,10 @@
         <v>10</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>191</v>
+        <v>347</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>192</v>
+        <v>348</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -4518,10 +4640,10 @@
         <v>10</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>189</v>
+        <v>349</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>190</v>
+        <v>350</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -4529,10 +4651,10 @@
         <v>10</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>187</v>
+        <v>351</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>188</v>
+        <v>352</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -4540,10 +4662,10 @@
         <v>10</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>185</v>
+        <v>353</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>186</v>
+        <v>354</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
@@ -4551,10 +4673,10 @@
         <v>10</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>183</v>
+        <v>355</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>184</v>
+        <v>356</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -4562,10 +4684,10 @@
         <v>10</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>182</v>
+        <v>357</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>182</v>
+        <v>358</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -4573,10 +4695,10 @@
         <v>10</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>180</v>
+        <v>359</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>181</v>
+        <v>360</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -4584,10 +4706,10 @@
         <v>10</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>178</v>
+        <v>361</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>179</v>
+        <v>362</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -4595,10 +4717,10 @@
         <v>10</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>176</v>
+        <v>363</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>177</v>
+        <v>364</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -4606,10 +4728,10 @@
         <v>10</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>174</v>
+        <v>365</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>175</v>
+        <v>366</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -4617,10 +4739,10 @@
         <v>10</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>172</v>
+        <v>367</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>173</v>
+        <v>368</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -4628,10 +4750,10 @@
         <v>10</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>170</v>
+        <v>369</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>171</v>
+        <v>370</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -4639,10 +4761,10 @@
         <v>10</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>168</v>
+        <v>371</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>169</v>
+        <v>372</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -4650,10 +4772,10 @@
         <v>10</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>166</v>
+        <v>373</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>167</v>
+        <v>374</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -4661,10 +4783,10 @@
         <v>10</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>164</v>
+        <v>387</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>165</v>
+        <v>388</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -4672,10 +4794,10 @@
         <v>10</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>162</v>
+        <v>389</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>163</v>
+        <v>390</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -4683,10 +4805,10 @@
         <v>10</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>160</v>
+        <v>391</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>161</v>
+        <v>392</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -4694,10 +4816,10 @@
         <v>10</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>158</v>
+        <v>393</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>159</v>
+        <v>394</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -4705,10 +4827,10 @@
         <v>10</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>156</v>
+        <v>395</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>157</v>
+        <v>396</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -4716,10 +4838,10 @@
         <v>10</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>154</v>
+        <v>397</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>155</v>
+        <v>398</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -4727,10 +4849,10 @@
         <v>10</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>152</v>
+        <v>399</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>153</v>
+        <v>400</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -4738,10 +4860,10 @@
         <v>10</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>150</v>
+        <v>401</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>151</v>
+        <v>402</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -4749,10 +4871,10 @@
         <v>10</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>148</v>
+        <v>403</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>149</v>
+        <v>404</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -4760,10 +4882,10 @@
         <v>10</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>146</v>
+        <v>405</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>147</v>
+        <v>406</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -4771,10 +4893,10 @@
         <v>10</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>144</v>
+        <v>407</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>145</v>
+        <v>408</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -4782,10 +4904,10 @@
         <v>10</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>142</v>
+        <v>409</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>143</v>
+        <v>410</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -4793,65 +4915,65 @@
         <v>10</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>140</v>
+        <v>411</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>141</v>
+        <v>412</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
-        <v>417</v>
+        <v>10</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="B213" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="C213" s="4" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B214" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="C214" s="4" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B215" s="5" t="s">
-        <v>428</v>
+      <c r="B215" s="4" t="s">
+        <v>418</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>641</v>
+        <v>419</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
-        <v>4</v>
+        <v>417</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>485</v>
+        <v>420</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>486</v>
+        <v>421</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -4859,10 +4981,10 @@
         <v>4</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -4870,10 +4992,10 @@
         <v>4</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>491</v>
+        <v>426</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>492</v>
+        <v>427</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -4881,10 +5003,10 @@
         <v>4</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>489</v>
+        <v>428</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>490</v>
+        <v>648</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -4892,10 +5014,10 @@
         <v>4</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>487</v>
+        <v>429</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>488</v>
+        <v>649</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -4903,10 +5025,10 @@
         <v>4</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>483</v>
+        <v>430</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>484</v>
+        <v>431</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -4914,10 +5036,10 @@
         <v>4</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>481</v>
+        <v>432</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>482</v>
+        <v>433</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -4925,65 +5047,65 @@
         <v>4</v>
       </c>
       <c r="B223" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C223" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B225" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="C223" s="4" t="s">
+      <c r="C225" s="4" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A224" s="5" t="s">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B224" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="C224" s="4" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" s="5" t="s">
+      <c r="B226" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B225" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="C225" s="4" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A226" s="5" t="s">
+      <c r="B227" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B226" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="C226" s="4" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A227" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B227" s="5" t="s">
-        <v>471</v>
-      </c>
-      <c r="C227" s="4" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B228" s="5" t="s">
-        <v>453</v>
+      <c r="B228" s="4" t="s">
+        <v>440</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -4991,17 +5113,17 @@
         <v>4</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>642</v>
+        <v>442</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A230" s="5" t="s">
+      <c r="A230" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B230" s="5" t="s">
+      <c r="B230" s="4" t="s">
         <v>444</v>
       </c>
       <c r="C230" s="4" t="s">
@@ -5009,135 +5131,135 @@
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A231" s="5" t="s">
+      <c r="A231" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B231" s="5" t="s">
-        <v>436</v>
+      <c r="B231" s="4" t="s">
+        <v>449</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>437</v>
+        <v>450</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="5" t="s">
+      <c r="A232" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B232" s="5" t="s">
-        <v>442</v>
+      <c r="B232" s="4" t="s">
+        <v>469</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>443</v>
+        <v>470</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A233" s="5" t="s">
+      <c r="A233" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B233" s="5" t="s">
-        <v>440</v>
+      <c r="B233" s="4" t="s">
+        <v>471</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>441</v>
+        <v>472</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A234" s="5" t="s">
+      <c r="A234" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B234" s="5" t="s">
-        <v>438</v>
+      <c r="B234" s="4" t="s">
+        <v>465</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>439</v>
+        <v>650</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A235" s="5" t="s">
+      <c r="A235" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B235" s="5" t="s">
-        <v>434</v>
+      <c r="B235" s="4" t="s">
+        <v>466</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>435</v>
+        <v>651</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" s="5" t="s">
+      <c r="A236" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B236" s="5" t="s">
+      <c r="B236" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C236" s="4" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="C237" s="4" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B238" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="C236" s="4" t="s">
+      <c r="C238" s="4" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" s="5" t="s">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B237" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="C237" s="4" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="5" t="s">
+      <c r="B239" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B238" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="C238" s="4" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" s="5" t="s">
+      <c r="B240" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B239" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="C239" s="4" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" s="5" t="s">
+      <c r="B241" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="C241" s="4" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B240" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="C240" s="4" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A241" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B241" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="C241" s="4" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B242" s="5" t="s">
-        <v>426</v>
+      <c r="B242" s="4" t="s">
+        <v>481</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>427</v>
+        <v>482</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -5145,10 +5267,10 @@
         <v>4</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>423</v>
+        <v>484</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -5156,10 +5278,10 @@
         <v>4</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>455</v>
+        <v>485</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>456</v>
+        <v>486</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -5167,10 +5289,10 @@
         <v>4</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>457</v>
+        <v>422</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>458</v>
+        <v>423</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -5178,10 +5300,10 @@
         <v>4</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>459</v>
+        <v>424</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>460</v>
+        <v>425</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -5189,10 +5311,10 @@
         <v>4</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -5200,10 +5322,10 @@
         <v>4</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>463</v>
+        <v>654</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -5211,10 +5333,10 @@
         <v>4</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -5222,10 +5344,10 @@
         <v>4</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>468</v>
+        <v>434</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>643</v>
+        <v>435</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -5233,10 +5355,10 @@
         <v>4</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>644</v>
+        <v>462</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -5244,10 +5366,10 @@
         <v>4</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>645</v>
+        <v>464</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -5255,131 +5377,131 @@
         <v>4</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>646</v>
+        <v>456</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>511</v>
+        <v>457</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>512</v>
+        <v>458</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>507</v>
+        <v>459</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>508</v>
+        <v>460</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>509</v>
+        <v>475</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>510</v>
+        <v>476</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>497</v>
+        <v>515</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>498</v>
+        <v>516</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>504</v>
+        <v>520</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>501</v>
+        <v>521</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>502</v>
+        <v>522</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>499</v>
+        <v>523</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>500</v>
+        <v>524</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>496</v>
+        <v>527</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>496</v>
+        <v>528</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>495</v>
+        <v>529</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>495</v>
+        <v>530</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -5387,10 +5509,10 @@
         <v>6</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>569</v>
+        <v>531</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>570</v>
+        <v>532</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -5398,10 +5520,10 @@
         <v>6</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>567</v>
+        <v>533</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>568</v>
+        <v>534</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -5409,10 +5531,10 @@
         <v>6</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>562</v>
+        <v>536</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -5420,10 +5542,10 @@
         <v>6</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -5431,10 +5553,10 @@
         <v>6</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>529</v>
+        <v>539</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>530</v>
+        <v>540</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -5464,10 +5586,10 @@
         <v>6</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>566</v>
+        <v>546</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -5475,10 +5597,10 @@
         <v>6</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>563</v>
+        <v>547</v>
       </c>
       <c r="C273" s="4" t="s">
-        <v>564</v>
+        <v>548</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -5486,10 +5608,10 @@
         <v>6</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="C274" s="4" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -5497,10 +5619,10 @@
         <v>6</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -5508,10 +5630,10 @@
         <v>6</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -5519,10 +5641,10 @@
         <v>6</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -5530,10 +5652,10 @@
         <v>6</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>550</v>
+        <v>558</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -5541,10 +5663,10 @@
         <v>6</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>545</v>
+        <v>561</v>
       </c>
       <c r="C279" s="4" t="s">
-        <v>546</v>
+        <v>562</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -5552,10 +5674,10 @@
         <v>6</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>539</v>
+        <v>563</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>540</v>
+        <v>564</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -5563,10 +5685,10 @@
         <v>6</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>537</v>
+        <v>565</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>538</v>
+        <v>566</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -5574,10 +5696,10 @@
         <v>6</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>535</v>
+        <v>567</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>536</v>
+        <v>568</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -5585,10 +5707,10 @@
         <v>6</v>
       </c>
       <c r="B283" s="4" t="s">
-        <v>531</v>
+        <v>569</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>532</v>
+        <v>570</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -5596,109 +5718,109 @@
         <v>6</v>
       </c>
       <c r="B284" s="4" t="s">
-        <v>527</v>
+        <v>559</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>528</v>
+        <v>560</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B285" s="4" t="s">
-        <v>525</v>
+        <v>655</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>526</v>
+        <v>656</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A286" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B286" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="C286" s="4" t="s">
-        <v>552</v>
+      <c r="A286" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B286" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="C286" s="6" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A287" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B287" s="4" t="s">
-        <v>547</v>
-      </c>
-      <c r="C287" s="4" t="s">
-        <v>548</v>
+      <c r="A287" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B287" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="C287" s="6" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>523</v>
+        <v>659</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>524</v>
+        <v>660</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>521</v>
+        <v>661</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>522</v>
+        <v>662</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B290" s="4" t="s">
-        <v>519</v>
+        <v>571</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>520</v>
+        <v>572</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B291" s="4" t="s">
-        <v>517</v>
+        <v>663</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>518</v>
+        <v>664</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>515</v>
+        <v>665</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>516</v>
+        <v>666</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A293" s="4" t="s">
+      <c r="A293" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B293" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="C293" s="4" t="s">
-        <v>576</v>
+      <c r="B293" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="C293" s="6" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -5717,98 +5839,98 @@
         <v>22</v>
       </c>
       <c r="B295" s="4" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="C295" s="4" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A296" s="6" t="s">
+      <c r="A296" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B296" s="6" t="s">
-        <v>647</v>
-      </c>
-      <c r="C296" s="6" t="s">
-        <v>648</v>
+      <c r="B296" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="C296" s="4" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A297" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B297" s="4" t="s">
-        <v>630</v>
-      </c>
-      <c r="C297" s="4" t="s">
-        <v>631</v>
+      <c r="A297" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B297" s="6" t="s">
+        <v>671</v>
+      </c>
+      <c r="C297" s="6" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>628</v>
+        <v>673</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>629</v>
+        <v>674</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B299" s="4" t="s">
-        <v>624</v>
+        <v>675</v>
       </c>
       <c r="C299" s="4" t="s">
-        <v>625</v>
+        <v>676</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B300" s="4" t="s">
-        <v>626</v>
+        <v>677</v>
       </c>
       <c r="C300" s="4" t="s">
-        <v>627</v>
+        <v>678</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B301" s="4" t="s">
-        <v>618</v>
+        <v>679</v>
       </c>
       <c r="C301" s="4" t="s">
-        <v>619</v>
+        <v>680</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B302" s="4" t="s">
-        <v>622</v>
+        <v>681</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>623</v>
+        <v>682</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>620</v>
+        <v>683</v>
       </c>
       <c r="C303" s="4" t="s">
-        <v>621</v>
+        <v>684</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -5816,10 +5938,10 @@
         <v>8</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>634</v>
+        <v>577</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>635</v>
+        <v>578</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -5827,10 +5949,10 @@
         <v>8</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>616</v>
+        <v>579</v>
       </c>
       <c r="C305" s="4" t="s">
-        <v>617</v>
+        <v>580</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -5838,10 +5960,10 @@
         <v>8</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
       <c r="C306" s="4" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -5849,10 +5971,10 @@
         <v>8</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>612</v>
+        <v>583</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>613</v>
+        <v>584</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -5860,10 +5982,10 @@
         <v>8</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>606</v>
+        <v>585</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>607</v>
+        <v>586</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -5871,10 +5993,10 @@
         <v>8</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>604</v>
+        <v>587</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>605</v>
+        <v>588</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -5882,10 +6004,10 @@
         <v>8</v>
       </c>
       <c r="B310" s="4" t="s">
-        <v>603</v>
+        <v>589</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>419</v>
+        <v>590</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -5893,10 +6015,10 @@
         <v>8</v>
       </c>
       <c r="B311" s="4" t="s">
-        <v>632</v>
+        <v>591</v>
       </c>
       <c r="C311" s="4" t="s">
-        <v>633</v>
+        <v>592</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -5904,10 +6026,10 @@
         <v>8</v>
       </c>
       <c r="B312" s="4" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>578</v>
+        <v>594</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -5926,10 +6048,10 @@
         <v>8</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="C314" s="4" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -5948,10 +6070,10 @@
         <v>8</v>
       </c>
       <c r="B316" s="4" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="C316" s="4" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -5959,10 +6081,10 @@
         <v>8</v>
       </c>
       <c r="B317" s="4" t="s">
-        <v>593</v>
+        <v>603</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>594</v>
+        <v>419</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -5970,10 +6092,10 @@
         <v>8</v>
       </c>
       <c r="B318" s="4" t="s">
-        <v>591</v>
+        <v>604</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>592</v>
+        <v>605</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -5981,10 +6103,10 @@
         <v>8</v>
       </c>
       <c r="B319" s="4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -5992,10 +6114,10 @@
         <v>8</v>
       </c>
       <c r="B320" s="4" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -6003,10 +6125,10 @@
         <v>8</v>
       </c>
       <c r="B321" s="4" t="s">
-        <v>589</v>
+        <v>610</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>590</v>
+        <v>611</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -6014,10 +6136,10 @@
         <v>8</v>
       </c>
       <c r="B322" s="4" t="s">
-        <v>587</v>
+        <v>614</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>588</v>
+        <v>615</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -6025,10 +6147,10 @@
         <v>8</v>
       </c>
       <c r="B323" s="4" t="s">
-        <v>585</v>
+        <v>616</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>586</v>
+        <v>617</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -6036,10 +6158,10 @@
         <v>8</v>
       </c>
       <c r="B324" s="4" t="s">
-        <v>583</v>
+        <v>618</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>584</v>
+        <v>619</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -6047,10 +6169,10 @@
         <v>8</v>
       </c>
       <c r="B325" s="4" t="s">
-        <v>581</v>
+        <v>620</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>582</v>
+        <v>621</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -6058,10 +6180,87 @@
         <v>8</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>579</v>
+        <v>622</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>580</v>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A327" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B327" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="C327" s="4" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B328" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="C328" s="4" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A329" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B329" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="C329" s="4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A330" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B330" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="C330" s="4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A331" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B331" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="C331" s="4" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A332" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B332" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="C332" s="4" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A333" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B333" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="C333" s="4" t="s">
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -6070,12 +6269,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6284,15 +6480,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15C6466F-2EDB-42B2-A93F-B216580033B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49965807-DF4C-4342-9D52-41238DAFCF90}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6317,10 +6517,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49965807-DF4C-4342-9D52-41238DAFCF90}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15C6466F-2EDB-42B2-A93F-B216580033B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>